<commit_message>
Modified sensitivity to use ProblemSpec
</commit_message>
<xml_diff>
--- a/tests/test_optimize/test_optimize.xlsx
+++ b/tests/test_optimize/test_optimize.xlsx
@@ -460,16 +460,16 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>5.086535652009559</v>
+        <v>4.739369273631283</v>
       </c>
       <c r="C2" t="n">
-        <v>5.105642372444731</v>
+        <v>4.733806412751601</v>
       </c>
       <c r="D2" t="n">
-        <v>61.85345770006964</v>
+        <v>459.0342543959424</v>
       </c>
       <c r="E2" t="n">
-        <v>0.01014932933619324</v>
+        <v>0.01137594362591159</v>
       </c>
     </row>
     <row r="3">
@@ -477,16 +477,16 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>5.086535652009559</v>
+        <v>4.739369273631283</v>
       </c>
       <c r="C3" t="n">
-        <v>5.105642372444731</v>
+        <v>4.733806412751601</v>
       </c>
       <c r="D3" t="n">
-        <v>61.85345770006964</v>
+        <v>459.0342543959424</v>
       </c>
       <c r="E3" t="n">
-        <v>0.008251313914658632</v>
+        <v>0.01072878202702245</v>
       </c>
     </row>
     <row r="4">
@@ -494,16 +494,16 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>5.086535652009559</v>
+        <v>4.977612155374525</v>
       </c>
       <c r="C4" t="n">
-        <v>5.105642372444731</v>
+        <v>4.958776757284687</v>
       </c>
       <c r="D4" t="n">
-        <v>61.85345770006964</v>
+        <v>7.247728239222934</v>
       </c>
       <c r="E4" t="n">
-        <v>0.009780911938579512</v>
+        <v>0.008927012830482495</v>
       </c>
     </row>
     <row r="5">
@@ -511,16 +511,16 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>4.87862744225316</v>
+        <v>4.977612155374525</v>
       </c>
       <c r="C5" t="n">
-        <v>4.961747398776303</v>
+        <v>4.958776757284687</v>
       </c>
       <c r="D5" t="n">
-        <v>53.50327458056672</v>
+        <v>7.247728239222934</v>
       </c>
       <c r="E5" t="n">
-        <v>0.009270709380359827</v>
+        <v>0.005790581315374009</v>
       </c>
     </row>
     <row r="6">
@@ -528,16 +528,16 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>4.87862744225316</v>
+        <v>4.977612155374525</v>
       </c>
       <c r="C6" t="n">
-        <v>4.961747398776303</v>
+        <v>4.958776757284687</v>
       </c>
       <c r="D6" t="n">
-        <v>53.50327458056672</v>
+        <v>7.247728239222934</v>
       </c>
       <c r="E6" t="n">
-        <v>0.008087735745107391</v>
+        <v>0.003464691520643704</v>
       </c>
     </row>
     <row r="7">
@@ -545,16 +545,16 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>4.87862744225316</v>
+        <v>4.977612155374525</v>
       </c>
       <c r="C7" t="n">
-        <v>4.961747398776303</v>
+        <v>4.958776757284687</v>
       </c>
       <c r="D7" t="n">
-        <v>53.50327458056672</v>
+        <v>7.247728239222934</v>
       </c>
       <c r="E7" t="n">
-        <v>0.01411640065900515</v>
+        <v>0.009663225338040772</v>
       </c>
     </row>
     <row r="8">
@@ -562,16 +562,16 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>4.87862744225316</v>
+        <v>4.968584659228433</v>
       </c>
       <c r="C8" t="n">
-        <v>4.961747398776303</v>
+        <v>4.988778195936124</v>
       </c>
       <c r="D8" t="n">
-        <v>53.50327458056672</v>
+        <v>3.661022268609827</v>
       </c>
       <c r="E8" t="n">
-        <v>0.01441254098089181</v>
+        <v>0.00990851032948474</v>
       </c>
     </row>
     <row r="9">
@@ -579,16 +579,16 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>5.000924348379161</v>
+        <v>4.975250419765318</v>
       </c>
       <c r="C9" t="n">
-        <v>5.046390088487067</v>
+        <v>4.993348893247816</v>
       </c>
       <c r="D9" t="n">
-        <v>7.161084629755707</v>
+        <v>2.15872358669173</v>
       </c>
       <c r="E9" t="n">
-        <v>0.01282566024057911</v>
+        <v>0.009580593045533901</v>
       </c>
     </row>
     <row r="10">
@@ -596,16 +596,16 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>5.03453018859206</v>
+        <v>4.975250419765318</v>
       </c>
       <c r="C10" t="n">
-        <v>5.026401776748363</v>
+        <v>4.993348893247816</v>
       </c>
       <c r="D10" t="n">
-        <v>6.297931936411532</v>
+        <v>2.15872358669173</v>
       </c>
       <c r="E10" t="n">
-        <v>0.01233985447896754</v>
+        <v>0.01096138785588309</v>
       </c>
     </row>
     <row r="11">
@@ -613,16 +613,16 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>4.991488441139264</v>
+        <v>4.975250419765318</v>
       </c>
       <c r="C11" t="n">
-        <v>4.960819172847855</v>
+        <v>4.993348893247816</v>
       </c>
       <c r="D11" t="n">
-        <v>5.295193462384429</v>
+        <v>2.15872358669173</v>
       </c>
       <c r="E11" t="n">
-        <v>0.01267618789684372</v>
+        <v>0.01052400080951986</v>
       </c>
     </row>
     <row r="12">
@@ -630,16 +630,16 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>4.991488441139264</v>
+        <v>4.986390794584488</v>
       </c>
       <c r="C12" t="n">
-        <v>4.960819172847855</v>
+        <v>5.014277080453552</v>
       </c>
       <c r="D12" t="n">
-        <v>5.295193462384429</v>
+        <v>1.293141969754038</v>
       </c>
       <c r="E12" t="n">
-        <v>0.01150579622466428</v>
+        <v>0.008854183951754073</v>
       </c>
     </row>
     <row r="13">
@@ -647,16 +647,16 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>5.005352325271297</v>
+        <v>4.993383311261053</v>
       </c>
       <c r="C13" t="n">
-        <v>4.994523496081769</v>
+        <v>4.993348893247816</v>
       </c>
       <c r="D13" t="n">
-        <v>0.1991185037490878</v>
+        <v>0.2879137868798451</v>
       </c>
       <c r="E13" t="n">
-        <v>0.008662383711674462</v>
+        <v>0.01151609599376997</v>
       </c>
     </row>
     <row r="14">
@@ -664,16 +664,16 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>5.000995375790023</v>
+        <v>4.991681653200199</v>
       </c>
       <c r="C14" t="n">
-        <v>5.007459349081508</v>
+        <v>4.998228616194902</v>
       </c>
       <c r="D14" t="n">
-        <v>0.1980060391732389</v>
+        <v>0.2380379360960141</v>
       </c>
       <c r="E14" t="n">
-        <v>0.006806002732663709</v>
+        <v>0.01092924081609513</v>
       </c>
     </row>
     <row r="15">
@@ -681,16 +681,16 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>5.000995375790023</v>
+        <v>5.000250444920759</v>
       </c>
       <c r="C15" t="n">
-        <v>5.007459349081508</v>
+        <v>5.000280965979282</v>
       </c>
       <c r="D15" t="n">
-        <v>0.1980060391732389</v>
+        <v>0.005935663731419322</v>
       </c>
       <c r="E15" t="n">
-        <v>0.009208179007787547</v>
+        <v>0.006993530024554418</v>
       </c>
     </row>
     <row r="16">
@@ -698,16 +698,16 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>4.997692625545517</v>
+        <v>4.999967104180334</v>
       </c>
       <c r="C16" t="n">
-        <v>4.996925997694882</v>
+        <v>5.00025966044814</v>
       </c>
       <c r="D16" t="n">
-        <v>0.05056006386998777</v>
+        <v>0.005497475709185652</v>
       </c>
       <c r="E16" t="n">
-        <v>0.008709559387526504</v>
+        <v>0.007351238293140759</v>
       </c>
     </row>
     <row r="17">
@@ -715,16 +715,16 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>4.998283170881029</v>
+        <v>4.999967104180334</v>
       </c>
       <c r="C17" t="n">
-        <v>4.998184343631356</v>
+        <v>5.00025966044814</v>
       </c>
       <c r="D17" t="n">
-        <v>0.02351888481966303</v>
+        <v>0.005497475709185652</v>
       </c>
       <c r="E17" t="n">
-        <v>0.01201552327579224</v>
+        <v>0.008268206027352856</v>
       </c>
     </row>
     <row r="18">
@@ -732,16 +732,16 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>4.997928598353852</v>
+        <v>4.999967104180334</v>
       </c>
       <c r="C18" t="n">
-        <v>4.999580075169306</v>
+        <v>5.00025966044814</v>
       </c>
       <c r="D18" t="n">
-        <v>0.0183066543506587</v>
+        <v>0.005497475709185652</v>
       </c>
       <c r="E18" t="n">
-        <v>0.01018696400649697</v>
+        <v>0.004333873690907626</v>
       </c>
     </row>
     <row r="19">
@@ -749,16 +749,16 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>4.998392722814084</v>
+        <v>4.999967104180334</v>
       </c>
       <c r="C19" t="n">
-        <v>5.000585811043651</v>
+        <v>5.00025966044814</v>
       </c>
       <c r="D19" t="n">
-        <v>0.01415328086493816</v>
+        <v>0.005497475709185652</v>
       </c>
       <c r="E19" t="n">
-        <v>0.01303160960439206</v>
+        <v>0.006154916302306768</v>
       </c>
     </row>
     <row r="20">
@@ -766,16 +766,16 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>4.998577010876718</v>
+        <v>5.000126848365561</v>
       </c>
       <c r="C20" t="n">
-        <v>5.000077502915837</v>
+        <v>4.99974426857862</v>
       </c>
       <c r="D20" t="n">
-        <v>0.01098076371123542</v>
+        <v>0.005311591277877292</v>
       </c>
       <c r="E20" t="n">
-        <v>0.02121762447867632</v>
+        <v>0.004474406245892526</v>
       </c>
     </row>
     <row r="21">
@@ -783,16 +783,16 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>5.000317773402267</v>
+        <v>4.999978002107094</v>
       </c>
       <c r="C21" t="n">
-        <v>5.000179728857832</v>
+        <v>4.999697872214196</v>
       </c>
       <c r="D21" t="n">
-        <v>0.005886098418824167</v>
+        <v>0.005219978598075844</v>
       </c>
       <c r="E21" t="n">
-        <v>0.01488624255479492</v>
+        <v>0.01207370020522915</v>
       </c>
     </row>
     <row r="22">
@@ -800,16 +800,16 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>5.000013369376668</v>
+        <v>4.999970928302389</v>
       </c>
       <c r="C22" t="n">
-        <v>4.999936225615375</v>
+        <v>5.000062526917813</v>
       </c>
       <c r="D22" t="n">
-        <v>0.005106443643546616</v>
+        <v>0.005162089461696572</v>
       </c>
       <c r="E22" t="n">
-        <v>0.01255613365441236</v>
+        <v>0.01612764977485064</v>
       </c>
     </row>
     <row r="23">
@@ -817,16 +817,16 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>5.000013369376668</v>
+        <v>4.999930523798098</v>
       </c>
       <c r="C23" t="n">
-        <v>4.999936225615375</v>
+        <v>4.999957042482018</v>
       </c>
       <c r="D23" t="n">
-        <v>0.005106443643546616</v>
+        <v>0.005074561432837549</v>
       </c>
       <c r="E23" t="n">
-        <v>0.01884255786210131</v>
+        <v>0.03004136544881693</v>
       </c>
     </row>
     <row r="24">
@@ -834,16 +834,16 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>4.999949838759657</v>
+        <v>4.999868308480597</v>
       </c>
       <c r="C24" t="n">
-        <v>4.999983432129614</v>
+        <v>4.999892108024093</v>
       </c>
       <c r="D24" t="n">
-        <v>0.005091123390829788</v>
+        <v>0.005066590317342493</v>
       </c>
       <c r="E24" t="n">
-        <v>0.1299527495281582</v>
+        <v>0.2148146314007081</v>
       </c>
     </row>
     <row r="25">
@@ -851,16 +851,16 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>4.999886084013236</v>
+        <v>4.99993827929849</v>
       </c>
       <c r="C25" t="n">
-        <v>4.999928145772652</v>
+        <v>4.999905950516123</v>
       </c>
       <c r="D25" t="n">
-        <v>0.00506532729974645</v>
+        <v>0.005066476609897517</v>
       </c>
       <c r="E25" t="n">
-        <v>0.6663442524539505</v>
+        <v>0.5542038037109747</v>
       </c>
     </row>
     <row r="26">
@@ -868,16 +868,16 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>4.999886084013236</v>
+        <v>4.999893700006857</v>
       </c>
       <c r="C26" t="n">
-        <v>4.999928145772652</v>
+        <v>4.999897131289655</v>
       </c>
       <c r="D26" t="n">
-        <v>0.00506532729974645</v>
+        <v>0.00506265596631361</v>
       </c>
       <c r="E26" t="n">
-        <v>2.141836383787513</v>
+        <v>2.014531456672368</v>
       </c>
     </row>
   </sheetData>

</xml_diff>